<commit_message>
ajouter du texte à la derniere section VerbNet
j'ai rajouté du texte dans la section juste avant la section Python
</commit_message>
<xml_diff>
--- a/echeancier.xlsx
+++ b/echeancier.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chapitre 1" sheetId="1" r:id="rId1"/>
-    <sheet name="diathese-lexique" sheetId="2" r:id="rId2"/>
+    <sheet name="chapitre 2" sheetId="3" r:id="rId2"/>
+    <sheet name="diathese-lexique" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'chapitre 1'!$A$1:$B$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'diathese-lexique'!$A$1:$B$982</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'diathese-lexique'!$A$1:$B$982</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="993">
   <si>
     <t>les pages</t>
   </si>
@@ -3005,6 +3006,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>p.35-40</t>
   </si>
 </sst>
 </file>
@@ -3357,10 +3361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3415,6 +3419,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>992</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3422,6 +3431,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B982"/>
   <sheetViews>

</xml_diff>

<commit_message>
modifié la structure du mémoire
</commit_message>
<xml_diff>
--- a/echeancier.xlsx
+++ b/echeancier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="chapitre 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="996">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="996">
   <si>
     <t>les pages</t>
   </si>
@@ -3373,8 +3373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3439,8 +3439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3456,9 +3456,6 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>989</v>
-      </c>
-      <c r="B2" t="s">
-        <v>987</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>